<commit_message>
disable half band filter
</commit_message>
<xml_diff>
--- a/cma_8000_3_1.xlsx
+++ b/cma_8000_3_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/multi-decode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F03FE81-A385-BB46-B15D-6AEEFBEB7C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3612F7-6C0C-A84E-A8CC-DD6A13C8BCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,16 +50,16 @@
     <t>db</t>
   </si>
   <si>
-    <t>Track 1, 16000 Hz</t>
+    <t>Track 1</t>
   </si>
   <si>
-    <t>Track 2, 16000 Hz</t>
+    <t>Track 2</t>
   </si>
   <si>
-    <t>Equalized AWGN, 16000 Hz, 0.02dB SNR per packet</t>
+    <t>Equalized AWGN, 0.02dB SNR per packet</t>
   </si>
   <si>
-    <t>De-Emphasized AWGN, 16000 Hz, 0.02 dB SNR per packet</t>
+    <t>De-Emphasized AWGN, 0.02 dB SNR per packet</t>
   </si>
 </sst>
 </file>
@@ -5897,8 +5897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3B20BF-DD24-9B45-85EB-8DC1C87F0292}">
   <dimension ref="B1:N152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10363,7 +10363,7 @@
         <v>332</v>
       </c>
       <c r="J132">
-        <f t="shared" ref="J132:J195" si="4">-($I$3*0.02)+(I132*0.02)</f>
+        <f t="shared" ref="J132:J152" si="4">-($I$3*0.02)+(I132*0.02)</f>
         <v>-0.55999999999999961</v>
       </c>
       <c r="L132">
@@ -10373,7 +10373,7 @@
         <v>359</v>
       </c>
       <c r="N132">
-        <f t="shared" ref="N132:N195" si="5">-($I$3*0.02)+(M132*0.02)</f>
+        <f t="shared" ref="N132:N152" si="5">-($I$3*0.02)+(M132*0.02)</f>
         <v>-2.0000000000000462E-2</v>
       </c>
     </row>

</xml_diff>